<commit_message>
review the whole tutorial and found many errors
Former-commit-id: c434ee0797213cac2fb84850036b076433158967
</commit_message>
<xml_diff>
--- a/iheadwater_hackweek_tutorials/data/pre_test_new.xlsx
+++ b/iheadwater_hackweek_tutorials/data/pre_test_new.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -717,60 +717,6 @@
         <v>1.1</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>北洛河大荔站</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1990-06-18</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>18:00:00</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2.1</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>北洛河大荔站</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1990-06-19</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>18:00:00</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2.2</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>